<commit_message>
Final module done and Budget project done! ZTM Excel course done!
</commit_message>
<xml_diff>
--- a/BUDGET_Excel_Project/BUDGET_PROJECT.xlsx
+++ b/BUDGET_Excel_Project/BUDGET_PROJECT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\Data Science\ZTM_Excel_Mastery\BUDGET_Excel_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8096163B-E6DB-48CB-82DF-AFEFD1908A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9737A64-5B87-4C3F-AF1F-D9F351D682C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="927" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="927" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Calc" sheetId="1" r:id="rId1"/>
@@ -870,6 +870,21 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -884,12 +899,6 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -912,15 +921,6 @@
     <xf numFmtId="10" fontId="9" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -931,6 +931,21 @@
     <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/mm/dd"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -950,21 +965,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/mm/dd"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -22081,7 +22081,7 @@
   <autoFilter ref="A1:B17" xr:uid="{FD8F80D2-6B3E-4977-8157-B4E49F48A6F3}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{FFBF28C0-71E3-44BE-8D52-02925852382C}" name="Category"/>
-    <tableColumn id="2" xr3:uid="{D82F61F4-4A0A-4932-ABCA-13E126ED13E3}" name="$ Spent" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{D82F61F4-4A0A-4932-ABCA-13E126ED13E3}" name="$ Spent" dataDxfId="4">
       <calculatedColumnFormula>SUMIFS(Trxn_History_Table[Debit], Trxn_History_Table[Category], Spend_Summary_Table[[#This Row],[Category]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -22093,11 +22093,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E5CF99D0-F9B7-42EE-9EB8-09FD136618B4}" name="Trxn_History_Table" displayName="Trxn_History_Table" ref="A1:E2327" totalsRowShown="0" headerRowCellStyle="Accent5">
   <autoFilter ref="A1:E2327" xr:uid="{E5CF99D0-F9B7-42EE-9EB8-09FD136618B4}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FF2B37D8-93DA-4DC1-BAAF-082605D9CCE4}" name="PurchaseDate" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{FF2B37D8-93DA-4DC1-BAAF-082605D9CCE4}" name="PurchaseDate" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{95945FAF-4E27-4CD8-8BB5-E407CF0D9985}" name="Description"/>
     <tableColumn id="3" xr3:uid="{37B629E0-36D8-47E8-929E-2B1A0E460562}" name="Category"/>
     <tableColumn id="4" xr3:uid="{CDA44DBB-8A6E-41BF-857C-81D4A56C74FD}" name="Debit"/>
-    <tableColumn id="5" xr3:uid="{4A8F03F8-FC18-44D2-A235-8D863A58DD7F}" name="CategoryGroup" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{4A8F03F8-FC18-44D2-A235-8D863A58DD7F}" name="CategoryGroup" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(Trxn_History_Table[[#This Row],[Category]],Trxn_Ctgry_Grp_Lookup[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -22109,8 +22109,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E8160EA8-28CA-427F-ACCB-C5FAD9E20AFF}" name="Trxn_Ctgry_Grp_Lookup" displayName="Trxn_Ctgry_Grp_Lookup" ref="A1:B17" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B17" xr:uid="{E8160EA8-28CA-427F-ACCB-C5FAD9E20AFF}"/>
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{8097E1A6-07FD-497A-B5DD-7ABF0A8042E3}" uniqueName="3" name="Subcategory" queryTableFieldId="3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E2BA66F8-E041-439C-A31A-2911905A2224}" uniqueName="4" name="Category" queryTableFieldId="4" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{8097E1A6-07FD-497A-B5DD-7ABF0A8042E3}" uniqueName="3" name="Subcategory" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{E2BA66F8-E041-439C-A31A-2911905A2224}" uniqueName="4" name="Category" queryTableFieldId="4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -22379,6 +22379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -22489,7 +22490,7 @@
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D8 D10">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22501,6 +22502,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDDA511-CA9E-44E0-98C3-4DCE5DDBD969}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -22659,6 +22661,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769DB53D-0AAC-4644-8617-4C476A4CF40D}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22714,6 +22717,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E94264-42BD-47F2-AF08-57474E473BB2}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22849,6 +22853,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2383BEB5-BBAF-43B5-BACD-CE422F08E9FE}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -22879,8 +22884,8 @@
     <row r="3" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="37"/>
       <c r="C3" s="38"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="44"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -22891,11 +22896,11 @@
         <v>93</v>
       </c>
       <c r="C4" s="40"/>
-      <c r="D4" s="57">
+      <c r="D4" s="45">
         <f>'Savings Goal Linked Cells (H)'!A2*1000</f>
         <v>53000</v>
       </c>
-      <c r="E4" s="57"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -22904,8 +22909,8 @@
     <row r="5" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B5" s="29"/>
       <c r="C5" s="30"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -22916,21 +22921,21 @@
         <v>94</v>
       </c>
       <c r="C6" s="40"/>
-      <c r="D6" s="44">
+      <c r="D6" s="49">
         <f ca="1">DATE(YEAR(TODAY()), MONTH(TODAY())+'Savings Goal Linked Cells (H)'!B2, DAY(TODAY()))</f>
         <v>47211</v>
       </c>
-      <c r="E6" s="44"/>
+      <c r="E6" s="49"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="12"/>
     </row>
     <row r="7" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="47"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -22941,20 +22946,20 @@
         <v>95</v>
       </c>
       <c r="C8" s="40"/>
-      <c r="D8" s="45">
+      <c r="D8" s="50">
         <v>3750</v>
       </c>
-      <c r="E8" s="45"/>
+      <c r="E8" s="50"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="12"/>
     </row>
     <row r="9" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B9" s="50"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="47"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -22965,11 +22970,11 @@
         <v>96</v>
       </c>
       <c r="C10" s="32"/>
-      <c r="D10" s="43">
+      <c r="D10" s="48">
         <f ca="1">(Svngs_Goal_Inp-Cur_Svngs_Inp)/DATEDIF(TODAY(), Trgt_Svngs_Date_Inp, "M")</f>
         <v>572.67441860465112</v>
       </c>
-      <c r="E10" s="43"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="8"/>
       <c r="G10" s="11" t="s">
         <v>98</v>
@@ -22980,10 +22985,10 @@
       <c r="I10" s="12"/>
     </row>
     <row r="11" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B11" s="52"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="47"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -22994,11 +22999,11 @@
         <v>97</v>
       </c>
       <c r="C12" s="32"/>
-      <c r="D12" s="54">
+      <c r="D12" s="57">
         <f ca="1">IF(Tot_Mnthly_Inc_Inp&gt;0, Mnthly_Svngs_Needed_Out/Tot_Mnthly_Inc_Inp, "0 or less Total Monthly Income")</f>
         <v>7.5292455772370648E-2</v>
       </c>
-      <c r="E12" s="54"/>
+      <c r="E12" s="57"/>
       <c r="F12" s="8"/>
       <c r="G12" s="11" t="s">
         <v>102</v>
@@ -23012,8 +23017,8 @@
     <row r="13" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="33"/>
       <c r="C13" s="34"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="42"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="47"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -23021,13 +23026,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="B10:C10"/>
@@ -23044,9 +23042,16 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23114,6 +23119,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63738CA-DCA2-4031-A665-6A49C51F0E5A}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23149,6 +23155,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A532210-BA0B-4A66-B604-B320D8DFFF95}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23182,6 +23189,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517B74DB-4983-42F8-ADCD-041BE9523AEC}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23359,9 +23367,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B9A8AD-860A-4E05-8772-5D88DD696769}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="B7:M39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
@@ -24518,9 +24527,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224E40E2-FE54-4FAF-9537-95269AC4597A}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:E2327"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:E2327"/>
     </sheetView>

</xml_diff>